<commit_message>
Order book time parameters
Fix log files location
</commit_message>
<xml_diff>
--- a/DataStructuresGeneration.xlsx
+++ b/DataStructuresGeneration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="17220" windowHeight="6888" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="17220" windowHeight="6888" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="496">
   <si>
     <t xml:space="preserve">public </t>
   </si>
@@ -1620,6 +1620,12 @@
   </si>
   <si>
     <t>1000 empty transaction specs with nulls</t>
+  </si>
+  <si>
+    <t>with nulls</t>
+  </si>
+  <si>
+    <t>without nulls</t>
   </si>
 </sst>
 </file>
@@ -7238,10 +7244,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7754,6 +7760,40 @@
       <c r="B42" s="10">
         <f>B41/F41-1</f>
         <v>-0.28898382667073552</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>494</v>
+      </c>
+      <c r="E46" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>10000</v>
+      </c>
+      <c r="E47">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>2225</v>
+      </c>
+      <c r="E48">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f>C48/C47</f>
+        <v>0.2225</v>
+      </c>
+      <c r="E49">
+        <f>E48/E47</f>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7779,8 +7819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView topLeftCell="E79" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>